<commit_message>
clear formatting from TemplateWithoutVBA.xlsx file
</commit_message>
<xml_diff>
--- a/Template_Without_VBA/TemplateWithoutVBA.xlsx
+++ b/Template_Without_VBA/TemplateWithoutVBA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SAPDevelop\Excel_Templates\Template_Without_VBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CE7A16-F5E0-4E45-8699-4C4A58F8103D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5540184A-07F1-4C81-9ED2-CAD176FFA494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3615" yWindow="-16560" windowWidth="38700" windowHeight="15345" tabRatio="374" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="12645" tabRatio="374" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SAP IBP Formatting Sheet" sheetId="14" state="hidden" r:id="rId1"/>
@@ -1199,69 +1199,6 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1286,6 +1223,69 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
@@ -1538,7 +1538,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>66675</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>342900</xdr:rowOff>
         </xdr:to>
@@ -2025,7 +2025,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>66675</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>342900</xdr:rowOff>
         </xdr:to>
@@ -3340,7 +3340,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>66675</xdr:colOff>
           <xdr:row>72</xdr:row>
           <xdr:rowOff>342900</xdr:rowOff>
         </xdr:to>
@@ -5708,19 +5708,19 @@
   <sheetData>
     <row r="1" spans="1:17" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
@@ -5770,43 +5770,43 @@
     </row>
     <row r="5" spans="1:17" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
-      <c r="L5" s="78"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="59"/>
       <c r="Q5" s="19" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="79"/>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="80"/>
-      <c r="G6" s="80"/>
-      <c r="H6" s="80"/>
-      <c r="I6" s="80"/>
-      <c r="J6" s="80"/>
-      <c r="K6" s="80"/>
-      <c r="L6" s="81"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="61"/>
+      <c r="L6" s="62"/>
       <c r="Q6" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="63" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="15"/>
@@ -5819,13 +5819,13 @@
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
       <c r="L7" s="16"/>
-      <c r="Q7" s="74" t="s">
+      <c r="Q7" s="66" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
-      <c r="B8" s="57"/>
+      <c r="B8" s="64"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -5836,35 +5836,35 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="10"/>
-      <c r="Q8" s="74"/>
+      <c r="Q8" s="66"/>
     </row>
     <row r="9" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
-      <c r="B9" s="57"/>
+      <c r="B9" s="64"/>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="59" t="s">
+      <c r="E9" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="60"/>
-      <c r="G9" s="61"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="69"/>
       <c r="H9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="59" t="s">
+      <c r="I9" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="60"/>
-      <c r="K9" s="61"/>
+      <c r="J9" s="68"/>
+      <c r="K9" s="69"/>
       <c r="L9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="Q9" s="74"/>
+      <c r="Q9" s="66"/>
     </row>
     <row r="10" spans="1:17" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="B10" s="57"/>
-      <c r="C10" s="62"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="2"/>
       <c r="E10" s="34"/>
       <c r="F10" s="34"/>
@@ -5874,12 +5874,12 @@
       <c r="J10" s="34"/>
       <c r="K10" s="34"/>
       <c r="L10" s="10"/>
-      <c r="Q10" s="74"/>
+      <c r="Q10" s="66"/>
     </row>
     <row r="11" spans="1:17" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="63"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="71"/>
       <c r="D11" s="35" t="s">
         <v>8</v>
       </c>
@@ -5899,12 +5899,12 @@
       <c r="L11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Q11" s="74"/>
+      <c r="Q11" s="66"/>
     </row>
     <row r="12" spans="1:17" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="65"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="72"/>
       <c r="D12" s="13"/>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
@@ -5914,11 +5914,11 @@
       <c r="J12" s="18"/>
       <c r="K12" s="18"/>
       <c r="L12" s="14"/>
-      <c r="Q12" s="74"/>
+      <c r="Q12" s="66"/>
     </row>
     <row r="13" spans="1:17" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="73" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="2"/>
@@ -5931,11 +5931,11 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="10"/>
-      <c r="Q13" s="74"/>
+      <c r="Q13" s="66"/>
     </row>
     <row r="14" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
-      <c r="B14" s="57"/>
+      <c r="B14" s="64"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -5946,35 +5946,35 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="10"/>
-      <c r="Q14" s="74"/>
+      <c r="Q14" s="66"/>
     </row>
     <row r="15" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
-      <c r="B15" s="57"/>
+      <c r="B15" s="64"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="59" t="s">
+      <c r="E15" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="60"/>
-      <c r="G15" s="61"/>
+      <c r="F15" s="68"/>
+      <c r="G15" s="69"/>
       <c r="H15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="59" t="s">
+      <c r="I15" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="60"/>
-      <c r="K15" s="61"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="69"/>
       <c r="L15" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="Q15" s="74"/>
+      <c r="Q15" s="66"/>
     </row>
     <row r="16" spans="1:17" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="62"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="70"/>
       <c r="D16" s="2"/>
       <c r="E16" s="34"/>
       <c r="F16" s="34"/>
@@ -5984,12 +5984,12 @@
       <c r="J16" s="34"/>
       <c r="K16" s="34"/>
       <c r="L16" s="10"/>
-      <c r="Q16" s="74"/>
+      <c r="Q16" s="66"/>
     </row>
     <row r="17" spans="1:17" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="63"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="71"/>
       <c r="D17" s="35" t="s">
         <v>8</v>
       </c>
@@ -6009,12 +6009,12 @@
       <c r="L17" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="Q17" s="74"/>
+      <c r="Q17" s="66"/>
     </row>
     <row r="18" spans="1:17" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="58"/>
-      <c r="C18" s="65"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="72"/>
       <c r="D18" s="13"/>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
@@ -6024,7 +6024,7 @@
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
       <c r="L18" s="14"/>
-      <c r="Q18" s="74"/>
+      <c r="Q18" s="66"/>
     </row>
     <row r="19" spans="1:17" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
@@ -6039,7 +6039,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-      <c r="Q19" s="74"/>
+      <c r="Q19" s="66"/>
     </row>
     <row r="20" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
@@ -6058,43 +6058,43 @@
     </row>
     <row r="21" spans="1:17" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
-      <c r="B21" s="66" t="s">
+      <c r="B21" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="67"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="67"/>
-      <c r="H21" s="67"/>
-      <c r="I21" s="67"/>
-      <c r="J21" s="67"/>
-      <c r="K21" s="67"/>
-      <c r="L21" s="68"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="75"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="75"/>
+      <c r="I21" s="75"/>
+      <c r="J21" s="75"/>
+      <c r="K21" s="75"/>
+      <c r="L21" s="76"/>
       <c r="Q21" s="22" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
-      <c r="B22" s="69"/>
-      <c r="C22" s="70"/>
-      <c r="D22" s="70"/>
-      <c r="E22" s="70"/>
-      <c r="F22" s="70"/>
-      <c r="G22" s="70"/>
-      <c r="H22" s="70"/>
-      <c r="I22" s="70"/>
-      <c r="J22" s="70"/>
-      <c r="K22" s="70"/>
-      <c r="L22" s="71"/>
-      <c r="Q22" s="74" t="s">
+      <c r="B22" s="77"/>
+      <c r="C22" s="78"/>
+      <c r="D22" s="78"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="78"/>
+      <c r="I22" s="78"/>
+      <c r="J22" s="78"/>
+      <c r="K22" s="78"/>
+      <c r="L22" s="79"/>
+      <c r="Q22" s="66" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
-      <c r="B23" s="56" t="s">
+      <c r="B23" s="73" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="2"/>
@@ -6107,35 +6107,35 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="10"/>
-      <c r="Q23" s="74"/>
+      <c r="Q23" s="66"/>
     </row>
     <row r="24" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
-      <c r="B24" s="57"/>
+      <c r="B24" s="64"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="59" t="s">
+      <c r="E24" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="60"/>
-      <c r="G24" s="61"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="69"/>
       <c r="H24" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I24" s="59" t="s">
+      <c r="I24" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="J24" s="60"/>
-      <c r="K24" s="61"/>
+      <c r="J24" s="68"/>
+      <c r="K24" s="69"/>
       <c r="L24" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="Q24" s="74"/>
+      <c r="Q24" s="66"/>
     </row>
     <row r="25" spans="1:17" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="62"/>
+      <c r="B25" s="64"/>
+      <c r="C25" s="70"/>
       <c r="D25" s="2"/>
       <c r="E25" s="34"/>
       <c r="F25" s="34"/>
@@ -6145,12 +6145,12 @@
       <c r="J25" s="34"/>
       <c r="K25" s="34"/>
       <c r="L25" s="10"/>
-      <c r="Q25" s="74"/>
+      <c r="Q25" s="66"/>
     </row>
     <row r="26" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="63"/>
+      <c r="B26" s="64"/>
+      <c r="C26" s="71"/>
       <c r="D26" s="35" t="s">
         <v>14</v>
       </c>
@@ -6170,12 +6170,12 @@
       <c r="L26" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Q26" s="74"/>
+      <c r="Q26" s="66"/>
     </row>
     <row r="27" spans="1:17" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
-      <c r="B27" s="57"/>
-      <c r="C27" s="64"/>
+      <c r="B27" s="64"/>
+      <c r="C27" s="80"/>
       <c r="D27" s="52"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
@@ -6185,12 +6185,12 @@
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
       <c r="L27" s="53"/>
-      <c r="Q27" s="74"/>
+      <c r="Q27" s="66"/>
     </row>
     <row r="28" spans="1:17" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
-      <c r="B28" s="57"/>
-      <c r="C28" s="63"/>
+      <c r="B28" s="64"/>
+      <c r="C28" s="71"/>
       <c r="D28" s="2"/>
       <c r="E28" s="34"/>
       <c r="F28" s="34"/>
@@ -6200,12 +6200,12 @@
       <c r="J28" s="34"/>
       <c r="K28" s="34"/>
       <c r="L28" s="10"/>
-      <c r="Q28" s="74"/>
+      <c r="Q28" s="66"/>
     </row>
     <row r="29" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
-      <c r="B29" s="57"/>
-      <c r="C29" s="63"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="71"/>
       <c r="D29" s="35" t="s">
         <v>15</v>
       </c>
@@ -6225,12 +6225,12 @@
       <c r="L29" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="Q29" s="74"/>
+      <c r="Q29" s="66"/>
     </row>
     <row r="30" spans="1:17" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="64"/>
+      <c r="B30" s="64"/>
+      <c r="C30" s="80"/>
       <c r="D30" s="52"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -6244,8 +6244,8 @@
     </row>
     <row r="31" spans="1:17" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="63"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="71"/>
       <c r="D31" s="2"/>
       <c r="E31" s="34"/>
       <c r="F31" s="34"/>
@@ -6258,8 +6258,8 @@
     </row>
     <row r="32" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
-      <c r="B32" s="57"/>
-      <c r="C32" s="63"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="71"/>
       <c r="D32" s="35" t="s">
         <v>37</v>
       </c>
@@ -6282,8 +6282,8 @@
     </row>
     <row r="33" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
-      <c r="B33" s="57"/>
-      <c r="C33" s="64"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="80"/>
       <c r="D33" s="52"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -6296,8 +6296,8 @@
     </row>
     <row r="34" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
-      <c r="B34" s="57"/>
-      <c r="C34" s="63"/>
+      <c r="B34" s="64"/>
+      <c r="C34" s="71"/>
       <c r="D34" s="2"/>
       <c r="E34" s="34"/>
       <c r="F34" s="34"/>
@@ -6310,8 +6310,8 @@
     </row>
     <row r="35" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
-      <c r="B35" s="57"/>
-      <c r="C35" s="63"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="71"/>
       <c r="D35" s="35" t="s">
         <v>31</v>
       </c>
@@ -6334,8 +6334,8 @@
     </row>
     <row r="36" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
-      <c r="B36" s="57"/>
-      <c r="C36" s="64"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="80"/>
       <c r="D36" s="52"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -6348,8 +6348,8 @@
     </row>
     <row r="37" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
-      <c r="B37" s="57"/>
-      <c r="C37" s="63"/>
+      <c r="B37" s="64"/>
+      <c r="C37" s="71"/>
       <c r="D37" s="2"/>
       <c r="E37" s="34"/>
       <c r="F37" s="34"/>
@@ -6362,8 +6362,8 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
-      <c r="B38" s="57"/>
-      <c r="C38" s="63"/>
+      <c r="B38" s="64"/>
+      <c r="C38" s="71"/>
       <c r="D38" s="35" t="s">
         <v>17</v>
       </c>
@@ -6378,7 +6378,7 @@
     </row>
     <row r="39" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
-      <c r="B39" s="57"/>
+      <c r="B39" s="64"/>
       <c r="C39" s="50"/>
       <c r="D39" s="35"/>
       <c r="E39" s="34"/>
@@ -6392,7 +6392,7 @@
     </row>
     <row r="40" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
-      <c r="B40" s="57"/>
+      <c r="B40" s="64"/>
       <c r="C40" s="50"/>
       <c r="D40" s="40" t="s">
         <v>18</v>
@@ -6416,7 +6416,7 @@
     </row>
     <row r="41" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
-      <c r="B41" s="57"/>
+      <c r="B41" s="64"/>
       <c r="C41" s="50"/>
       <c r="D41" s="31"/>
       <c r="E41" s="7"/>
@@ -6430,7 +6430,7 @@
     </row>
     <row r="42" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
-      <c r="B42" s="57"/>
+      <c r="B42" s="64"/>
       <c r="C42" s="50"/>
       <c r="D42" s="35"/>
       <c r="E42" s="34"/>
@@ -6444,7 +6444,7 @@
     </row>
     <row r="43" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
-      <c r="B43" s="57"/>
+      <c r="B43" s="64"/>
       <c r="C43" s="50"/>
       <c r="D43" s="40" t="s">
         <v>32</v>
@@ -6468,7 +6468,7 @@
     </row>
     <row r="44" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
-      <c r="B44" s="57"/>
+      <c r="B44" s="64"/>
       <c r="C44" s="50"/>
       <c r="D44" s="31"/>
       <c r="E44" s="7"/>
@@ -6482,7 +6482,7 @@
     </row>
     <row r="45" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
-      <c r="B45" s="57"/>
+      <c r="B45" s="64"/>
       <c r="C45" s="50"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -6496,7 +6496,7 @@
     </row>
     <row r="46" spans="1:12" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
-      <c r="B46" s="58"/>
+      <c r="B46" s="65"/>
       <c r="C46" s="51"/>
       <c r="D46" s="13"/>
       <c r="E46" s="13"/>
@@ -6510,7 +6510,7 @@
     </row>
     <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
-      <c r="B47" s="73" t="s">
+      <c r="B47" s="63" t="s">
         <v>4</v>
       </c>
       <c r="C47" s="15"/>
@@ -6526,30 +6526,30 @@
     </row>
     <row r="48" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
-      <c r="B48" s="57"/>
+      <c r="B48" s="64"/>
       <c r="C48" s="5"/>
       <c r="D48" s="6"/>
-      <c r="E48" s="59" t="s">
+      <c r="E48" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="F48" s="60"/>
-      <c r="G48" s="61"/>
+      <c r="F48" s="68"/>
+      <c r="G48" s="69"/>
       <c r="H48" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I48" s="59" t="s">
+      <c r="I48" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="J48" s="60"/>
-      <c r="K48" s="61"/>
+      <c r="J48" s="68"/>
+      <c r="K48" s="69"/>
       <c r="L48" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
-      <c r="B49" s="57"/>
-      <c r="C49" s="62"/>
+      <c r="B49" s="64"/>
+      <c r="C49" s="70"/>
       <c r="D49" s="2"/>
       <c r="E49" s="34"/>
       <c r="F49" s="34"/>
@@ -6562,8 +6562,8 @@
     </row>
     <row r="50" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
-      <c r="B50" s="57"/>
-      <c r="C50" s="63"/>
+      <c r="B50" s="64"/>
+      <c r="C50" s="71"/>
       <c r="D50" s="35" t="s">
         <v>14</v>
       </c>
@@ -6586,8 +6586,8 @@
     </row>
     <row r="51" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
-      <c r="B51" s="57"/>
-      <c r="C51" s="64"/>
+      <c r="B51" s="64"/>
+      <c r="C51" s="80"/>
       <c r="D51" s="52"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
@@ -6600,8 +6600,8 @@
     </row>
     <row r="52" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
-      <c r="B52" s="57"/>
-      <c r="C52" s="63"/>
+      <c r="B52" s="64"/>
+      <c r="C52" s="71"/>
       <c r="D52" s="2"/>
       <c r="E52" s="34"/>
       <c r="F52" s="34"/>
@@ -6614,8 +6614,8 @@
     </row>
     <row r="53" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
-      <c r="B53" s="57"/>
-      <c r="C53" s="63"/>
+      <c r="B53" s="64"/>
+      <c r="C53" s="71"/>
       <c r="D53" s="35" t="s">
         <v>15</v>
       </c>
@@ -6638,8 +6638,8 @@
     </row>
     <row r="54" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
-      <c r="B54" s="57"/>
-      <c r="C54" s="64"/>
+      <c r="B54" s="64"/>
+      <c r="C54" s="80"/>
       <c r="D54" s="52"/>
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
@@ -6652,8 +6652,8 @@
     </row>
     <row r="55" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
-      <c r="B55" s="57"/>
-      <c r="C55" s="63"/>
+      <c r="B55" s="64"/>
+      <c r="C55" s="71"/>
       <c r="D55" s="2"/>
       <c r="E55" s="34"/>
       <c r="F55" s="34"/>
@@ -6666,8 +6666,8 @@
     </row>
     <row r="56" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
-      <c r="B56" s="57"/>
-      <c r="C56" s="63"/>
+      <c r="B56" s="64"/>
+      <c r="C56" s="71"/>
       <c r="D56" s="35" t="s">
         <v>37</v>
       </c>
@@ -6690,8 +6690,8 @@
     </row>
     <row r="57" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
-      <c r="B57" s="57"/>
-      <c r="C57" s="64"/>
+      <c r="B57" s="64"/>
+      <c r="C57" s="80"/>
       <c r="D57" s="52"/>
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
@@ -6704,8 +6704,8 @@
     </row>
     <row r="58" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
-      <c r="B58" s="57"/>
-      <c r="C58" s="63"/>
+      <c r="B58" s="64"/>
+      <c r="C58" s="71"/>
       <c r="D58" s="2"/>
       <c r="E58" s="34"/>
       <c r="F58" s="34"/>
@@ -6718,8 +6718,8 @@
     </row>
     <row r="59" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
-      <c r="B59" s="57"/>
-      <c r="C59" s="63"/>
+      <c r="B59" s="64"/>
+      <c r="C59" s="71"/>
       <c r="D59" s="35" t="s">
         <v>31</v>
       </c>
@@ -6742,8 +6742,8 @@
     </row>
     <row r="60" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
-      <c r="B60" s="57"/>
-      <c r="C60" s="64"/>
+      <c r="B60" s="64"/>
+      <c r="C60" s="80"/>
       <c r="D60" s="52"/>
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
@@ -6756,8 +6756,8 @@
     </row>
     <row r="61" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
-      <c r="B61" s="57"/>
-      <c r="C61" s="63"/>
+      <c r="B61" s="64"/>
+      <c r="C61" s="71"/>
       <c r="D61" s="2"/>
       <c r="E61" s="34"/>
       <c r="F61" s="34"/>
@@ -6770,8 +6770,8 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
-      <c r="B62" s="57"/>
-      <c r="C62" s="63"/>
+      <c r="B62" s="64"/>
+      <c r="C62" s="71"/>
       <c r="D62" s="35" t="s">
         <v>17</v>
       </c>
@@ -6786,7 +6786,7 @@
     </row>
     <row r="63" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
-      <c r="B63" s="57"/>
+      <c r="B63" s="64"/>
       <c r="C63" s="50"/>
       <c r="D63" s="35"/>
       <c r="E63" s="34"/>
@@ -6800,7 +6800,7 @@
     </row>
     <row r="64" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
-      <c r="B64" s="57"/>
+      <c r="B64" s="64"/>
       <c r="C64" s="50"/>
       <c r="D64" s="40" t="s">
         <v>33</v>
@@ -6824,7 +6824,7 @@
     </row>
     <row r="65" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
-      <c r="B65" s="57"/>
+      <c r="B65" s="64"/>
       <c r="C65" s="50"/>
       <c r="D65" s="31"/>
       <c r="E65" s="7"/>
@@ -6838,7 +6838,7 @@
     </row>
     <row r="66" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
-      <c r="B66" s="57"/>
+      <c r="B66" s="64"/>
       <c r="C66" s="50"/>
       <c r="D66" s="35"/>
       <c r="E66" s="34"/>
@@ -6852,7 +6852,7 @@
     </row>
     <row r="67" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
-      <c r="B67" s="57"/>
+      <c r="B67" s="64"/>
       <c r="C67" s="50"/>
       <c r="D67" s="40" t="s">
         <v>34</v>
@@ -6876,7 +6876,7 @@
     </row>
     <row r="68" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
-      <c r="B68" s="57"/>
+      <c r="B68" s="64"/>
       <c r="C68" s="50"/>
       <c r="D68" s="31"/>
       <c r="E68" s="7"/>
@@ -6890,7 +6890,7 @@
     </row>
     <row r="69" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
-      <c r="B69" s="57"/>
+      <c r="B69" s="64"/>
       <c r="C69" s="50"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -6904,7 +6904,7 @@
     </row>
     <row r="70" spans="1:12" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
-      <c r="B70" s="58"/>
+      <c r="B70" s="65"/>
       <c r="C70" s="51"/>
       <c r="D70" s="13"/>
       <c r="E70" s="13"/>
@@ -6946,37 +6946,37 @@
     </row>
     <row r="73" spans="1:12" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
-      <c r="B73" s="66" t="s">
+      <c r="B73" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="C73" s="67"/>
-      <c r="D73" s="67"/>
-      <c r="E73" s="67"/>
-      <c r="F73" s="67"/>
-      <c r="G73" s="67"/>
-      <c r="H73" s="67"/>
-      <c r="I73" s="67"/>
-      <c r="J73" s="67"/>
-      <c r="K73" s="67"/>
-      <c r="L73" s="68"/>
+      <c r="C73" s="75"/>
+      <c r="D73" s="75"/>
+      <c r="E73" s="75"/>
+      <c r="F73" s="75"/>
+      <c r="G73" s="75"/>
+      <c r="H73" s="75"/>
+      <c r="I73" s="75"/>
+      <c r="J73" s="75"/>
+      <c r="K73" s="75"/>
+      <c r="L73" s="76"/>
     </row>
     <row r="74" spans="1:12" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2"/>
-      <c r="B74" s="69"/>
-      <c r="C74" s="70"/>
-      <c r="D74" s="70"/>
-      <c r="E74" s="70"/>
-      <c r="F74" s="70"/>
-      <c r="G74" s="70"/>
-      <c r="H74" s="70"/>
-      <c r="I74" s="70"/>
-      <c r="J74" s="70"/>
-      <c r="K74" s="70"/>
-      <c r="L74" s="71"/>
+      <c r="B74" s="77"/>
+      <c r="C74" s="78"/>
+      <c r="D74" s="78"/>
+      <c r="E74" s="78"/>
+      <c r="F74" s="78"/>
+      <c r="G74" s="78"/>
+      <c r="H74" s="78"/>
+      <c r="I74" s="78"/>
+      <c r="J74" s="78"/>
+      <c r="K74" s="78"/>
+      <c r="L74" s="79"/>
     </row>
     <row r="75" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
-      <c r="B75" s="56" t="s">
+      <c r="B75" s="73" t="s">
         <v>12</v>
       </c>
       <c r="C75" s="2"/>
@@ -6992,30 +6992,30 @@
     </row>
     <row r="76" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
-      <c r="B76" s="57"/>
+      <c r="B76" s="64"/>
       <c r="C76" s="5"/>
       <c r="D76" s="6"/>
-      <c r="E76" s="59" t="s">
+      <c r="E76" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="F76" s="60"/>
-      <c r="G76" s="61"/>
+      <c r="F76" s="68"/>
+      <c r="G76" s="69"/>
       <c r="H76" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I76" s="59" t="s">
+      <c r="I76" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="J76" s="60"/>
-      <c r="K76" s="61"/>
+      <c r="J76" s="68"/>
+      <c r="K76" s="69"/>
       <c r="L76" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2"/>
-      <c r="B77" s="57"/>
-      <c r="C77" s="62"/>
+      <c r="B77" s="64"/>
+      <c r="C77" s="70"/>
       <c r="D77" s="2"/>
       <c r="E77" s="34"/>
       <c r="F77" s="34"/>
@@ -7028,8 +7028,8 @@
     </row>
     <row r="78" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="2"/>
-      <c r="B78" s="57"/>
-      <c r="C78" s="63"/>
+      <c r="B78" s="64"/>
+      <c r="C78" s="71"/>
       <c r="D78" s="35" t="s">
         <v>21</v>
       </c>
@@ -7052,8 +7052,8 @@
     </row>
     <row r="79" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
-      <c r="B79" s="57"/>
-      <c r="C79" s="64"/>
+      <c r="B79" s="64"/>
+      <c r="C79" s="80"/>
       <c r="D79" s="52"/>
       <c r="E79" s="7"/>
       <c r="F79" s="7"/>
@@ -7066,8 +7066,8 @@
     </row>
     <row r="80" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2"/>
-      <c r="B80" s="57"/>
-      <c r="C80" s="63"/>
+      <c r="B80" s="64"/>
+      <c r="C80" s="71"/>
       <c r="D80" s="2"/>
       <c r="E80" s="34"/>
       <c r="F80" s="34"/>
@@ -7080,8 +7080,8 @@
     </row>
     <row r="81" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A81" s="2"/>
-      <c r="B81" s="57"/>
-      <c r="C81" s="63"/>
+      <c r="B81" s="64"/>
+      <c r="C81" s="71"/>
       <c r="D81" s="35" t="s">
         <v>22</v>
       </c>
@@ -7104,8 +7104,8 @@
     </row>
     <row r="82" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2"/>
-      <c r="B82" s="72"/>
-      <c r="C82" s="64"/>
+      <c r="B82" s="81"/>
+      <c r="C82" s="80"/>
       <c r="D82" s="52"/>
       <c r="E82" s="7"/>
       <c r="F82" s="7"/>
@@ -7118,7 +7118,7 @@
     </row>
     <row r="83" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2"/>
-      <c r="B83" s="56" t="s">
+      <c r="B83" s="73" t="s">
         <v>4</v>
       </c>
       <c r="C83" s="2"/>
@@ -7134,30 +7134,30 @@
     </row>
     <row r="84" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2"/>
-      <c r="B84" s="57"/>
+      <c r="B84" s="64"/>
       <c r="C84" s="5"/>
       <c r="D84" s="6"/>
-      <c r="E84" s="59" t="s">
+      <c r="E84" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="F84" s="60"/>
-      <c r="G84" s="61"/>
+      <c r="F84" s="68"/>
+      <c r="G84" s="69"/>
       <c r="H84" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I84" s="59" t="s">
+      <c r="I84" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="J84" s="60"/>
-      <c r="K84" s="61"/>
+      <c r="J84" s="68"/>
+      <c r="K84" s="69"/>
       <c r="L84" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="85" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2"/>
-      <c r="B85" s="57"/>
-      <c r="C85" s="62"/>
+      <c r="B85" s="64"/>
+      <c r="C85" s="70"/>
       <c r="D85" s="2"/>
       <c r="E85" s="34"/>
       <c r="F85" s="34"/>
@@ -7170,8 +7170,8 @@
     </row>
     <row r="86" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A86" s="2"/>
-      <c r="B86" s="57"/>
-      <c r="C86" s="63"/>
+      <c r="B86" s="64"/>
+      <c r="C86" s="71"/>
       <c r="D86" s="35" t="s">
         <v>21</v>
       </c>
@@ -7194,8 +7194,8 @@
     </row>
     <row r="87" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
-      <c r="B87" s="57"/>
-      <c r="C87" s="64"/>
+      <c r="B87" s="64"/>
+      <c r="C87" s="80"/>
       <c r="D87" s="52"/>
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
@@ -7208,8 +7208,8 @@
     </row>
     <row r="88" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2"/>
-      <c r="B88" s="57"/>
-      <c r="C88" s="63"/>
+      <c r="B88" s="64"/>
+      <c r="C88" s="71"/>
       <c r="D88" s="2"/>
       <c r="E88" s="34"/>
       <c r="F88" s="34"/>
@@ -7222,8 +7222,8 @@
     </row>
     <row r="89" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A89" s="2"/>
-      <c r="B89" s="57"/>
-      <c r="C89" s="63"/>
+      <c r="B89" s="64"/>
+      <c r="C89" s="71"/>
       <c r="D89" s="35" t="s">
         <v>22</v>
       </c>
@@ -7246,8 +7246,8 @@
     </row>
     <row r="90" spans="1:12" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
-      <c r="B90" s="58"/>
-      <c r="C90" s="65"/>
+      <c r="B90" s="65"/>
+      <c r="C90" s="72"/>
       <c r="D90" s="13"/>
       <c r="E90" s="18"/>
       <c r="F90" s="18"/>
@@ -8045,6 +8045,37 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="/Chmw4zSd3RJ1wMxaE3DbLzaXzujPt7FFSOhA/pH0mLBB1mHkoDZPXarzxdqU85i1j82PBx4Eb6X22eWPx1tJQ==" saltValue="Wv6Y+aUwtP+n2PtDScGYIg==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0"/>
   <mergeCells count="43">
+    <mergeCell ref="B83:B90"/>
+    <mergeCell ref="E84:G84"/>
+    <mergeCell ref="I84:K84"/>
+    <mergeCell ref="C85:C87"/>
+    <mergeCell ref="C88:C90"/>
+    <mergeCell ref="B75:B82"/>
+    <mergeCell ref="E76:G76"/>
+    <mergeCell ref="I76:K76"/>
+    <mergeCell ref="C77:C79"/>
+    <mergeCell ref="C80:C82"/>
+    <mergeCell ref="B47:B70"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="B73:L73"/>
+    <mergeCell ref="B74:L74"/>
+    <mergeCell ref="I48:K48"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="C52:C54"/>
+    <mergeCell ref="C55:C57"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="B21:L21"/>
+    <mergeCell ref="B22:L22"/>
+    <mergeCell ref="Q22:Q29"/>
+    <mergeCell ref="B23:B46"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="C37:C38"/>
     <mergeCell ref="B1:L1"/>
     <mergeCell ref="B5:L5"/>
     <mergeCell ref="B6:L6"/>
@@ -8057,37 +8088,6 @@
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="I15:K15"/>
     <mergeCell ref="C16:C18"/>
-    <mergeCell ref="B21:L21"/>
-    <mergeCell ref="B22:L22"/>
-    <mergeCell ref="Q22:Q29"/>
-    <mergeCell ref="B23:B46"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="I48:K48"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="C52:C54"/>
-    <mergeCell ref="C55:C57"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B47:B70"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="B73:L73"/>
-    <mergeCell ref="B74:L74"/>
-    <mergeCell ref="B75:B82"/>
-    <mergeCell ref="E76:G76"/>
-    <mergeCell ref="I76:K76"/>
-    <mergeCell ref="C77:C79"/>
-    <mergeCell ref="C80:C82"/>
-    <mergeCell ref="B83:B90"/>
-    <mergeCell ref="E84:G84"/>
-    <mergeCell ref="I84:K84"/>
-    <mergeCell ref="C85:C87"/>
-    <mergeCell ref="C88:C90"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8095,19 +8095,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="24577" r:id="rId3" name="cbApplyLevelFormatting">
+        <control shapeId="24599" r:id="rId3" name="cbApplyOddEvenFormatting">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" r:id="rId4">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>266700</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>72</xdr:row>
                 <xdr:rowOff>66675</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>66675</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>72</xdr:row>
                 <xdr:rowOff>342900</xdr:rowOff>
               </to>
             </anchor>
@@ -8115,13 +8115,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="24577" r:id="rId3" name="cbApplyLevelFormatting"/>
+        <control shapeId="24599" r:id="rId3" name="cbApplyOddEvenFormatting"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <control shapeId="24583" r:id="rId5" name="cbApplyMemberFormatting">
-          <controlPr defaultSize="0" autoFill="0" autoLine="0" r:id="rId4">
+          <controlPr defaultSize="0" autoFill="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
@@ -8145,19 +8145,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="24599" r:id="rId6" name="cbApplyOddEvenFormatting">
-          <controlPr defaultSize="0" autoFill="0" autoLine="0" r:id="rId7">
+        <control shapeId="24577" r:id="rId7" name="cbApplyLevelFormatting">
+          <controlPr defaultSize="0" autoFill="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>266700</xdr:colOff>
-                <xdr:row>72</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>66675</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>66675</xdr:colOff>
-                <xdr:row>72</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>342900</xdr:rowOff>
               </to>
             </anchor>
@@ -8165,7 +8165,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="24599" r:id="rId6" name="cbApplyOddEvenFormatting"/>
+        <control shapeId="24577" r:id="rId7" name="cbApplyLevelFormatting"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9124,11 +9124,11 @@
   <dimension ref="A1:CG6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="10" ySplit="5" topLeftCell="AZ1048556" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="5" topLeftCell="K6" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K6" sqref="K6"/>
       <selection pane="topRight" activeCell="K6" sqref="K6"/>
       <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
-      <selection pane="bottomRight" activeCell="K6" sqref="K6:CG1048576"/>
+      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9447,16 +9447,15 @@
   <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId1"/>
   <customProperties>
     <customPr name="EpmWorksheetKeyString_GUID" r:id="rId2"/>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId3"/>
   </customProperties>
-  <drawing r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
-  <picture r:id="rId6"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
+  <picture r:id="rId5"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="3093" r:id="rId7" name="FPMExcelClientSheetOptionstb1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
+        <control shapeId="3093" r:id="rId6" name="FPMExcelClientSheetOptionstb1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -9475,7 +9474,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="3093" r:id="rId7" name="FPMExcelClientSheetOptionstb1"/>
+        <control shapeId="3093" r:id="rId6" name="FPMExcelClientSheetOptionstb1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -9488,10 +9487,10 @@
   <dimension ref="A1:CG6"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="10" ySplit="5" topLeftCell="AZ1048556" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="5" topLeftCell="K6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="K6" sqref="K6:CG1048576"/>
+      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9810,16 +9809,40 @@
   <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId1"/>
   <customProperties>
     <customPr name="EpmWorksheetKeyString_GUID" r:id="rId2"/>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId3"/>
   </customProperties>
-  <drawing r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
-  <picture r:id="rId6"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
+  <picture r:id="rId5"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="5127" r:id="rId7" name="TextBox2">
-          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId8">
+        <control shapeId="5121" r:id="rId6" name="FPMExcelClientSheetOptionstb1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="5121" r:id="rId6" name="FPMExcelClientSheetOptionstb1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="5127" r:id="rId8" name="TextBox2">
+          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId9">
             <anchor>
               <from>
                 <xdr:col>8</xdr:col>
@@ -9838,32 +9861,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="5127" r:id="rId7" name="TextBox2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="5121" r:id="rId9" name="FPMExcelClientSheetOptionstb1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
-            <anchor moveWithCells="1" sizeWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="5121" r:id="rId9" name="FPMExcelClientSheetOptionstb1"/>
+        <control shapeId="5127" r:id="rId8" name="TextBox2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>